<commit_message>
Upload the final version
Test Completed
</commit_message>
<xml_diff>
--- a/subfunds_navs.xlsx
+++ b/subfunds_navs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\PycharmProjects\quantRiskDevTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william\Downloads\Inter view - Next\ngt_test-quant_risk_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA7F2E-106E-4369-8682-DAB31AD4A394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7B8C0F-5A58-4874-BA17-B99568651E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{50204325-77B7-4CF2-819B-CC7DCC22AB24}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{50204325-77B7-4CF2-819B-CC7DCC22AB24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{395462C9-8543-4D94-B72C-D9AB9128275C}" name="Table1" displayName="Table1" ref="A1:C1029" totalsRowShown="0">
-  <autoFilter ref="A1:C1029" xr:uid="{395462C9-8543-4D94-B72C-D9AB9128275C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BC56FB24-FDC8-4BB4-A695-DF08C7A11991}" name="Subfund_Code"/>
     <tableColumn id="2" xr3:uid="{1A9131AF-0172-4169-AAB2-A79C5E32916D}" name="Valuation_Date" dataDxfId="0"/>
@@ -428,7 +427,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FBD6F5-3760-4EA9-816E-135A1BE229F0}">
   <dimension ref="A1:C1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>